<commit_message>
Correct Former Owner column headings
</commit_message>
<xml_diff>
--- a/data/mmw-leaves-test.xlsx
+++ b/data/mmw-leaves-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/openn-genizah/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63B8A002-9E14-574B-AC19-36DECB8B0B44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19FE19C-AFFB-7A45-8264-691FF213B56F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{42E12B04-1FA5-BF45-9FB7-FDE600D8B5D6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Call Number/ID</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Language</t>
   </si>
   <si>
-    <t>Former Owner</t>
-  </si>
-  <si>
-    <t>FO Ref</t>
-  </si>
-  <si>
     <t>Manuscript Name</t>
   </si>
   <si>
@@ -132,86 +126,65 @@
     <t>Quran Leaves</t>
   </si>
   <si>
-    <t>Lewis C 6</t>
-  </si>
-  <si>
-    <t>lewis_c_006</t>
-  </si>
-  <si>
-    <t>mmw00005.tif|mmw00006.tif</t>
-  </si>
-  <si>
-    <t>Lewis C 6 front|Lewis C 6 reverse</t>
-  </si>
-  <si>
-    <t>23 x 17 cm</t>
-  </si>
-  <si>
-    <t>Lewis C 16</t>
-  </si>
-  <si>
-    <t>lewis_c_016</t>
-  </si>
-  <si>
-    <t>mmw00007.tif|mmw00008.tif</t>
-  </si>
-  <si>
-    <t>Lewis C 16 front|Lewis C 16 reverse</t>
-  </si>
-  <si>
-    <t>11.5 x 21 cm</t>
-  </si>
-  <si>
-    <t>Four Lines of Calligraphy from the Qasidat al-Burda</t>
-  </si>
-  <si>
-    <t>Lewis C 17</t>
-  </si>
-  <si>
-    <t>lewis_c_017</t>
-  </si>
-  <si>
-    <t>mmw00009.tif|mmw00010.tif</t>
-  </si>
-  <si>
-    <t>Lewis C 17 front|Lewis C 17 reverse</t>
-  </si>
-  <si>
-    <t>14 x 23 cm</t>
-  </si>
-  <si>
-    <t>Leaf from the Qasidat al-Burda</t>
-  </si>
-  <si>
-    <t>Lewis C 18</t>
-  </si>
-  <si>
-    <t>lewis_c_018</t>
-  </si>
-  <si>
-    <t>mmw00011.tif|mmw00012.tif</t>
-  </si>
-  <si>
-    <t>Lewis C 18 front|Lewis C 18 reverse</t>
-  </si>
-  <si>
-    <t>19.5 x 28.5 cm</t>
-  </si>
-  <si>
     <t>per</t>
   </si>
   <si>
-    <t>Persian Calligraphy in Cloudbands</t>
-  </si>
-  <si>
     <t>https://viaf.org/viaf/63874811</t>
+  </si>
+  <si>
+    <t>Former Owner name</t>
+  </si>
+  <si>
+    <t>Former Owner URI</t>
+  </si>
+  <si>
+    <t>Lewis M 27</t>
+  </si>
+  <si>
+    <t>lewis_m_027</t>
+  </si>
+  <si>
+    <t>mmw00057.tif|mmw00058.tif</t>
+  </si>
+  <si>
+    <t>Lewis M 27 front|Lewis M 27 reverse</t>
+  </si>
+  <si>
+    <t>17 x 30 cm</t>
+  </si>
+  <si>
+    <t>Exhibited at the Philadelphia Museum of Art, "The Book of War: The Free Library of Philadelphia's Mughal Razmnama Folios July 14, 2007 - December 9, 2007"</t>
+  </si>
+  <si>
+    <t>Razmnama Leaf, The Cloud Kundadhara Bestows Virtue on a Brahman; Razmnama Leaf</t>
+  </si>
+  <si>
+    <t>Lewis M 74</t>
+  </si>
+  <si>
+    <t>lewis_m_074</t>
+  </si>
+  <si>
+    <t>mmw00085.tif|mmw00086.tif</t>
+  </si>
+  <si>
+    <t>Lewis M 74 front|Lewis M 74 reverse</t>
+  </si>
+  <si>
+    <t>20.5 x 32 cm</t>
+  </si>
+  <si>
+    <t>Previously attributed to the painter Mansur in the Mughal court of Jahangir.|Signed by 17th-century court calligrapher 'Abd al-Rahim 'Anbarin Qalam.</t>
+  </si>
+  <si>
+    <t>Painting of a Horned Pheasant; Verses from the Divan-i-Hafiz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,6 +196,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -248,9 +229,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,11 +547,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DCCD94-56E9-804A-8F49-F586F84B7573}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,260 +590,184 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" t="s">
-        <v>56</v>
-      </c>
       <c r="N5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
         <v>47</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>